<commit_message>
Add new form, update models, and modify project files
- Added `Test.cs`, `Test.Designer.cs`, and `Test.resx` to `MainForms.csproj`.
- Added `clDatatypes.cs` to `Models.csproj` and removed from `Utilities.csproj`.
- Fixed formatting issue in `clConnection.cs` exception message.
- Updated `clInteractDb.cs` to modify SQLite and SQL Server table creation queries and include `UserId` in `Users` table `INSERT` statement.
- Added new form `Test` in `MainForms` namespace with event handlers and controls.
- Implemented `clDatatypes` class for SQL query conversion based on database type.
- Updated binary file `MediMax.xlsx`.
</commit_message>
<xml_diff>
--- a/MediMax.xlsx
+++ b/MediMax.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="175">
   <si>
     <t xml:space="preserve">Sr.</t>
   </si>
@@ -502,31 +502,52 @@
     <t xml:space="preserve">Date and time of the error.</t>
   </si>
   <si>
-    <t xml:space="preserve">Comparison Between SQLite and SQL Server Data Types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary Key</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INTEGER PRIMARY KEY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VARCHAR(X)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Float/Numeric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boolean</t>
+    <t xml:space="preserve">Custom Type Marker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Express Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQLite Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_V_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_V_[50]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_D_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_T_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_B_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_S_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_I_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_N_[20?2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMERIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECIMAL(p,s)</t>
   </si>
 </sst>
 </file>
@@ -535,14 +556,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0;[RED]\-#,##0"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00;\-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0;[RED]\-#,##0"/>
   </numFmts>
   <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -560,17 +582,19 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFC0C0C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC0C0C0"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -604,23 +628,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6E6"/>
-        <bgColor rgb="FFE6E6FF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -636,8 +655,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6E6"/>
+        <bgColor rgb="FFE6E6FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDDE8CB"/>
         <bgColor rgb="FFE6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
   </fills>
@@ -645,62 +676,6 @@
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair">
-        <color rgb="FF000080"/>
-      </right>
-      <top style="hair">
-        <color rgb="FF000080"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair">
-        <color rgb="FF000080"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair">
-        <color rgb="FF000080"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -740,6 +715,55 @@
       <left style="hair">
         <color rgb="FF000080"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair">
+        <color rgb="FF000080"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair">
+        <color rgb="FF000080"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000080"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FF000080"/>
+      </left>
       <right style="hair">
         <color rgb="FF000080"/>
       </right>
@@ -749,6 +773,13 @@
       <bottom style="hair">
         <color rgb="FF000080"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -783,48 +814,48 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="10" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -845,27 +876,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -877,19 +912,19 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Result2" xfId="20"/>
-    <cellStyle name="Background" xfId="21"/>
-    <cellStyle name="Card" xfId="22"/>
-    <cellStyle name="Input" xfId="23"/>
-    <cellStyle name="Card TL" xfId="24"/>
-    <cellStyle name="Card T" xfId="25"/>
-    <cellStyle name="Card TR" xfId="26"/>
-    <cellStyle name="Card L" xfId="27"/>
-    <cellStyle name="Card R" xfId="28"/>
-    <cellStyle name="Card B" xfId="29"/>
-    <cellStyle name="Card BL" xfId="30"/>
-    <cellStyle name="Card BR" xfId="31"/>
-    <cellStyle name="Column Header" xfId="32"/>
+    <cellStyle name="Background" xfId="20"/>
+    <cellStyle name="Card" xfId="21"/>
+    <cellStyle name="Card B" xfId="22"/>
+    <cellStyle name="Card BL" xfId="23"/>
+    <cellStyle name="Card BR" xfId="24"/>
+    <cellStyle name="Card L" xfId="25"/>
+    <cellStyle name="Card R" xfId="26"/>
+    <cellStyle name="Card T" xfId="27"/>
+    <cellStyle name="Card TL" xfId="28"/>
+    <cellStyle name="Card TR" xfId="29"/>
+    <cellStyle name="Column Header" xfId="30"/>
+    <cellStyle name="Input" xfId="31"/>
+    <cellStyle name="Result2" xfId="32"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -945,7 +980,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1133,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:H749"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="2" sqref="E22 G34 G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5261,8 +5296,8 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="2" sqref="E22 G34 N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5676,8 +5711,8 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="E22 G34 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5708,112 +5743,114 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:H77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="1" sqref="E22 G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="25.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="5" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="5" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="6"/>
@@ -5821,155 +5858,154 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="6"/>
@@ -5977,597 +6013,596 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="8"/>
+      <c r="G19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9" t="s">
+      <c r="D20" s="10"/>
+      <c r="E20" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9" t="s">
+      <c r="D21" s="10"/>
+      <c r="E21" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
+      <c r="D22" s="10"/>
+      <c r="E22" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9" t="s">
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9" t="s">
+      <c r="D25" s="10"/>
+      <c r="E25" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="6"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9" t="s">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="H27" s="6"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="H28" s="6"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9" t="s">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9" t="s">
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9" t="s">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="H31" s="6"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9" t="s">
+      <c r="D32" s="10"/>
+      <c r="E32" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9" t="s">
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9" t="s">
+      <c r="D33" s="10"/>
+      <c r="E33" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9" t="s">
+      <c r="F33" s="10"/>
+      <c r="G33" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="6"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9" t="s">
+      <c r="D34" s="10"/>
+      <c r="E34" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9" t="s">
+      <c r="F34" s="10"/>
+      <c r="G34" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="H34" s="6"/>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9" t="s">
+      <c r="D35" s="10"/>
+      <c r="E35" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9" t="s">
+      <c r="F35" s="10"/>
+      <c r="G35" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="H35" s="6"/>
+      <c r="H35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9" t="s">
+      <c r="D36" s="10"/>
+      <c r="E36" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="H36" s="6"/>
+      <c r="H36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9" t="s">
+      <c r="D37" s="10"/>
+      <c r="E37" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9" t="s">
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="H37" s="6"/>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9" t="s">
+      <c r="D38" s="10"/>
+      <c r="E38" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9" t="s">
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="H38" s="6"/>
+      <c r="H38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9" t="s">
+      <c r="D39" s="10"/>
+      <c r="E39" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="H39" s="6"/>
+      <c r="H39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9" t="s">
+      <c r="D40" s="10"/>
+      <c r="E40" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9" t="s">
+      <c r="F40" s="10"/>
+      <c r="G40" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="H40" s="6"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9" t="s">
+      <c r="D41" s="10"/>
+      <c r="E41" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9" t="s">
+      <c r="F41" s="10"/>
+      <c r="G41" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="H41" s="6"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9" t="s">
+      <c r="D42" s="10"/>
+      <c r="E42" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9" t="s">
+      <c r="F42" s="10"/>
+      <c r="G42" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="H42" s="6"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9" t="s">
+      <c r="D43" s="10"/>
+      <c r="E43" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9" t="s">
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="10"/>
     </row>
     <row r="44" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9" t="s">
+      <c r="D44" s="10"/>
+      <c r="E44" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9" t="s">
+      <c r="F44" s="10"/>
+      <c r="G44" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="H44" s="6"/>
+      <c r="H44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9" t="s">
+      <c r="D45" s="10"/>
+      <c r="E45" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9" t="s">
+      <c r="F45" s="10"/>
+      <c r="G45" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="H45" s="6"/>
+      <c r="H45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9" t="s">
+      <c r="D46" s="10"/>
+      <c r="E46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9" t="s">
+      <c r="F46" s="10"/>
+      <c r="G46" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="H46" s="6"/>
+      <c r="H46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9" t="s">
+      <c r="D47" s="10"/>
+      <c r="E47" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9" t="s">
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="H47" s="6"/>
+      <c r="H47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9" t="s">
+      <c r="D48" s="10"/>
+      <c r="E48" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9" t="s">
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="H48" s="6"/>
+      <c r="H48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9" t="s">
+      <c r="D49" s="10"/>
+      <c r="E49" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9" t="s">
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="H49" s="6"/>
+      <c r="H49" s="10"/>
     </row>
     <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9" t="s">
+      <c r="D50" s="10"/>
+      <c r="E50" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9" t="s">
+      <c r="F50" s="10"/>
+      <c r="G50" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="6"/>
+      <c r="H50" s="10"/>
     </row>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9" t="s">
+      <c r="D51" s="10"/>
+      <c r="E51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9" t="s">
+      <c r="F51" s="10"/>
+      <c r="G51" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="H51" s="6"/>
+      <c r="H51" s="10"/>
     </row>
     <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="9" t="s">
+      <c r="C52" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9" t="s">
+      <c r="D52" s="10"/>
+      <c r="E52" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9" t="s">
+      <c r="F52" s="10"/>
+      <c r="G52" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="H52" s="6"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="6"/>
@@ -6575,87 +6610,86 @@
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
       <c r="H53" s="6"/>
     </row>
     <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
       <c r="H54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7" t="s">
+      <c r="D55" s="8"/>
+      <c r="E55" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7" t="s">
+      <c r="F55" s="8"/>
+      <c r="G55" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H55" s="6"/>
+      <c r="H55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C56" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9" t="s">
+      <c r="D56" s="10"/>
+      <c r="E56" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9" t="s">
+      <c r="F56" s="10"/>
+      <c r="G56" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H56" s="6"/>
+      <c r="H56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="C57" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9" t="s">
+      <c r="D57" s="10"/>
+      <c r="E57" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9" t="s">
+      <c r="F57" s="10"/>
+      <c r="G57" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H57" s="6"/>
+      <c r="H57" s="10"/>
     </row>
     <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9" t="s">
+      <c r="D58" s="10"/>
+      <c r="E58" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9" t="s">
+      <c r="F58" s="10"/>
+      <c r="G58" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="H58" s="6"/>
+      <c r="H58" s="10"/>
     </row>
     <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="6"/>
@@ -6663,138 +6697,145 @@
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
       <c r="H59" s="6"/>
     </row>
     <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="5" t="s">
+      <c r="A60" s="11"/>
+      <c r="B60" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
       <c r="H60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="11"/>
+      <c r="B61" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7" t="s">
+      <c r="D61" s="8"/>
+      <c r="E61" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7" t="s">
+      <c r="F61" s="8"/>
+      <c r="G61" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H61" s="6"/>
+      <c r="H61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B62" s="8" t="s">
+      <c r="A62" s="11"/>
+      <c r="B62" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9" t="s">
+      <c r="D62" s="10"/>
+      <c r="E62" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F62" s="9"/>
-      <c r="G62" s="9" t="s">
+      <c r="F62" s="10"/>
+      <c r="G62" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="6"/>
+      <c r="H62" s="10"/>
     </row>
     <row r="63" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="9" t="s">
+      <c r="A63" s="11"/>
+      <c r="B63" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9" t="s">
+      <c r="D63" s="10"/>
+      <c r="E63" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9" t="s">
+      <c r="F63" s="10"/>
+      <c r="G63" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="H63" s="6"/>
+      <c r="H63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="9" t="s">
+      <c r="A64" s="11"/>
+      <c r="B64" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9" t="s">
+      <c r="D64" s="10"/>
+      <c r="E64" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9" t="s">
+      <c r="F64" s="10"/>
+      <c r="G64" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="H64" s="6"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="9" t="s">
+      <c r="A65" s="11"/>
+      <c r="B65" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9" t="s">
+      <c r="D65" s="10"/>
+      <c r="E65" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9" t="s">
+      <c r="F65" s="10"/>
+      <c r="G65" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H65" s="6"/>
+      <c r="H65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="9" t="s">
+      <c r="A66" s="11"/>
+      <c r="B66" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="9"/>
-      <c r="E66" s="9" t="s">
+      <c r="D66" s="10"/>
+      <c r="E66" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9" t="s">
+      <c r="F66" s="10"/>
+      <c r="G66" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="H66" s="6"/>
+      <c r="H66" s="10"/>
     </row>
     <row r="67" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="9" t="s">
+      <c r="A67" s="11"/>
+      <c r="B67" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9" t="s">
+      <c r="D67" s="10"/>
+      <c r="E67" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9" t="s">
+      <c r="F67" s="10"/>
+      <c r="G67" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="H67" s="6"/>
+      <c r="H67" s="10"/>
     </row>
     <row r="68" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="6"/>
@@ -6802,288 +6843,399 @@
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
       <c r="H68" s="6"/>
     </row>
     <row r="69" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="5" t="s">
+      <c r="A69" s="0"/>
+      <c r="B69" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="6"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="10"/>
+      <c r="A70" s="0"/>
+      <c r="B70" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I70" s="10"/>
     </row>
     <row r="71" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B71" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E71" s="9"/>
-      <c r="F71" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G71" s="9"/>
-      <c r="H71" s="10"/>
+      <c r="A71" s="0"/>
+      <c r="B71" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I71" s="10"/>
     </row>
     <row r="72" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B72" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G72" s="9"/>
-      <c r="H72" s="10"/>
+      <c r="A72" s="0"/>
+      <c r="B72" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I72" s="10"/>
     </row>
     <row r="73" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9" t="s">
+      <c r="A73" s="0"/>
+      <c r="B73" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I73" s="10"/>
+    </row>
+    <row r="74" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0"/>
+      <c r="B74" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I74" s="10"/>
+    </row>
+    <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0"/>
+      <c r="B75" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9" t="s">
+      <c r="I75" s="10"/>
+    </row>
+    <row r="76" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0"/>
+      <c r="B76" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="G73" s="9"/>
-      <c r="H73" s="10"/>
-    </row>
-    <row r="74" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9" t="s">
+      <c r="G76" s="10"/>
+      <c r="H76" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I76" s="10"/>
+    </row>
+    <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0"/>
+      <c r="B77" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G74" s="9"/>
-      <c r="H74" s="10"/>
-    </row>
-    <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B75" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="G75" s="9"/>
-      <c r="H75" s="10"/>
-    </row>
-    <row r="76" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B76" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C76" s="9"/>
-      <c r="D76" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G76" s="9"/>
-      <c r="H76" s="10"/>
-    </row>
-    <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G77" s="9"/>
-      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+    </row>
+    <row r="78" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="146">
+  <mergeCells count="215">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:H27"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:H29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:H37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:H41"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="E47:F47"/>
+    <mergeCell ref="G47:H47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="E50:F50"/>
+    <mergeCell ref="G50:H50"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="E51:F51"/>
+    <mergeCell ref="G51:H51"/>
     <mergeCell ref="C52:D52"/>
     <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
     <mergeCell ref="B54:G54"/>
     <mergeCell ref="C55:D55"/>
     <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="E57:F57"/>
+    <mergeCell ref="G57:H57"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="E58:F58"/>
+    <mergeCell ref="G58:H58"/>
     <mergeCell ref="B60:G60"/>
     <mergeCell ref="C61:D61"/>
     <mergeCell ref="E61:F61"/>
+    <mergeCell ref="G61:H61"/>
     <mergeCell ref="C62:D62"/>
     <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:H62"/>
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="E63:F63"/>
+    <mergeCell ref="G63:H63"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="E64:F64"/>
+    <mergeCell ref="G64:H64"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="E65:F65"/>
+    <mergeCell ref="G65:H65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="E67:F67"/>
-    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="H69:I69"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="F70:G70"/>
+    <mergeCell ref="H70:I70"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:I72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:E73"/>
     <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="D74:E74"/>
     <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H74:I74"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="F75:G75"/>
+    <mergeCell ref="H75:I75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
     <mergeCell ref="B77:C77"/>
     <mergeCell ref="D77:E77"/>
     <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="1.025" header="0.511811023622047" footer="0.7875"/>

</xml_diff>

<commit_message>
Update query placeholders and init methods for SQLite/SQLExpress
Updated `clDatatypes.cs` to replace `_T_` with `_DT_` for `DATETIME NOT NULL` and `_S_` with `_SI_` for `INTEGER NOT NULL` and `SMALLINT NOT NULL`. Modified `InitializeSQLiteDatabase` and `InitializeSQLExpressDatabase` in `clInteractDb.cs` to use `clDatatypes.ConvertQuery` for placeholder conversion. Added foreign key enabling and state data insertion for SQLite. Ensured consistent use of new placeholders and correct schema setup for both databases.
</commit_message>
<xml_diff>
--- a/MediMax.xlsx
+++ b/MediMax.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="dbMediMax" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Text Files" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Tables" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="States" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="246">
   <si>
     <t xml:space="preserve">Sr.</t>
   </si>
@@ -505,9 +506,6 @@
     <t xml:space="preserve">Custom Type Marker</t>
   </si>
   <si>
-    <t xml:space="preserve">Base Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">SQL Express Conversion</t>
   </si>
   <si>
@@ -517,9 +515,6 @@
     <t xml:space="preserve">_V_</t>
   </si>
   <si>
-    <t xml:space="preserve">VARCHAR</t>
-  </si>
-  <si>
     <t xml:space="preserve">VARCHAR(1)</t>
   </si>
   <si>
@@ -529,13 +524,13 @@
     <t xml:space="preserve">_D_</t>
   </si>
   <si>
-    <t xml:space="preserve">_T_</t>
+    <t xml:space="preserve">_DT_</t>
   </si>
   <si>
     <t xml:space="preserve">_B_</t>
   </si>
   <si>
-    <t xml:space="preserve">_S_</t>
+    <t xml:space="preserve">_SI_</t>
   </si>
   <si>
     <t xml:space="preserve">_I_</t>
@@ -544,20 +539,240 @@
     <t xml:space="preserve">_N_[20?2]</t>
   </si>
   <si>
-    <t xml:space="preserve">NUMERIC</t>
-  </si>
-  <si>
     <t xml:space="preserve">DECIMAL(p,s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jammu and Kashmir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Himachal Pradesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Punjab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandigarh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uttarakhand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haryana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajasthan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uttar Pradesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bihar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sikkim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nagaland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manipur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mizoram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tripura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meghalaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West Bengal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jharkhand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orissa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chhattisgarh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madhya Pradesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gujarat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daman and Diu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dadra and Nagar Haveli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maharashtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andhra Pradesh (Old)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karnataka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakshadweep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamil Nadu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puducherry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andaman and Nicobar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telengana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andhra Pradesh (New)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00;\-#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0;[RED]\-#,##0"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -855,7 +1070,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -874,10 +1089,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -900,7 +1111,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1168,7 +1391,7 @@
   </sheetPr>
   <dimension ref="A1:H749"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -5296,7 +5519,7 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
@@ -5711,7 +5934,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5745,1282 +5968,1224 @@
   </sheetPr>
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F82" activeCellId="0" sqref="F82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="25.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="5" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="12.9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="5" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="10"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="10"/>
-    </row>
-    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="10"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="10"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="10"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10" t="s">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="H14" s="10"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="8"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="10"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10" t="s">
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="10"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
+      <c r="F22" s="9"/>
+      <c r="G22" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="10"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10" t="s">
+      <c r="F23" s="9"/>
+      <c r="G23" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="10"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10" t="s">
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10" t="s">
+      <c r="F24" s="9"/>
+      <c r="G24" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="10"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10" t="s">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10" t="s">
+      <c r="F25" s="9"/>
+      <c r="G25" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="10"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10" t="s">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10" t="s">
+      <c r="F26" s="9"/>
+      <c r="G26" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="H26" s="10"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10" t="s">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10" t="s">
+      <c r="F27" s="9"/>
+      <c r="G27" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H27" s="10"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10" t="s">
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
+      <c r="F28" s="9"/>
+      <c r="G28" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H28" s="10"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10" t="s">
+      <c r="F29" s="9"/>
+      <c r="G29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="H29" s="10"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10" t="s">
+      <c r="F30" s="9"/>
+      <c r="G30" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H30" s="10"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10" t="s">
+      <c r="F31" s="9"/>
+      <c r="G31" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H31" s="10"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
+      <c r="F32" s="9"/>
+      <c r="G32" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H32" s="10"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10" t="s">
+      <c r="D33" s="9"/>
+      <c r="E33" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10" t="s">
+      <c r="F33" s="9"/>
+      <c r="G33" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H33" s="10"/>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10" t="s">
+      <c r="D34" s="9"/>
+      <c r="E34" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10" t="s">
+      <c r="F34" s="9"/>
+      <c r="G34" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="H34" s="10"/>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10" t="s">
+      <c r="D35" s="9"/>
+      <c r="E35" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10" t="s">
+      <c r="F35" s="9"/>
+      <c r="G35" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="H35" s="10"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10" t="s">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10" t="s">
+      <c r="F36" s="9"/>
+      <c r="G36" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="H36" s="10"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10" t="s">
+      <c r="D37" s="9"/>
+      <c r="E37" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10" t="s">
+      <c r="F37" s="9"/>
+      <c r="G37" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="H37" s="10"/>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10" t="s">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10" t="s">
+      <c r="F38" s="9"/>
+      <c r="G38" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="H38" s="10"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10" t="s">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10" t="s">
+      <c r="F39" s="9"/>
+      <c r="G39" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="H39" s="10"/>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10" t="s">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10" t="s">
+      <c r="F40" s="9"/>
+      <c r="G40" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="H40" s="10"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10" t="s">
+      <c r="D41" s="9"/>
+      <c r="E41" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10" t="s">
+      <c r="F41" s="9"/>
+      <c r="G41" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H41" s="10"/>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10" t="s">
+      <c r="D42" s="9"/>
+      <c r="E42" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10" t="s">
+      <c r="F42" s="9"/>
+      <c r="G42" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="H42" s="10"/>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10" t="s">
+      <c r="D43" s="9"/>
+      <c r="E43" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10" t="s">
+      <c r="F43" s="9"/>
+      <c r="G43" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="H43" s="10"/>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10" t="s">
+      <c r="D44" s="9"/>
+      <c r="E44" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10" t="s">
+      <c r="F44" s="9"/>
+      <c r="G44" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H44" s="10"/>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10" t="s">
+      <c r="D45" s="9"/>
+      <c r="E45" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10" t="s">
+      <c r="F45" s="9"/>
+      <c r="G45" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="H45" s="10"/>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10" t="s">
+      <c r="D46" s="9"/>
+      <c r="E46" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10" t="s">
+      <c r="F46" s="9"/>
+      <c r="G46" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="H46" s="10"/>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10" t="s">
+      <c r="D47" s="9"/>
+      <c r="E47" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10" t="s">
+      <c r="F47" s="9"/>
+      <c r="G47" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="H47" s="10"/>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10" t="s">
+      <c r="D48" s="9"/>
+      <c r="E48" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10" t="s">
+      <c r="F48" s="9"/>
+      <c r="G48" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H48" s="10"/>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10" t="s">
+      <c r="D49" s="9"/>
+      <c r="E49" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10" t="s">
+      <c r="F49" s="9"/>
+      <c r="G49" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="H49" s="10"/>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10" t="s">
+      <c r="D50" s="9"/>
+      <c r="E50" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10" t="s">
+      <c r="F50" s="9"/>
+      <c r="G50" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="H50" s="10"/>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10" t="s">
+      <c r="D51" s="9"/>
+      <c r="E51" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="10"/>
-      <c r="G51" s="10" t="s">
+      <c r="F51" s="9"/>
+      <c r="G51" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="H51" s="10"/>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10" t="s">
+      <c r="D52" s="9"/>
+      <c r="E52" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F52" s="10"/>
-      <c r="G52" s="10" t="s">
+      <c r="F52" s="9"/>
+      <c r="G52" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="H52" s="10"/>
-    </row>
-    <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="H53" s="6"/>
-    </row>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
     </row>
     <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8" t="s">
+      <c r="D55" s="7"/>
+      <c r="E55" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H55" s="8"/>
+      <c r="H55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10" t="s">
+      <c r="D56" s="9"/>
+      <c r="E56" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10" t="s">
+      <c r="F56" s="9"/>
+      <c r="G56" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="H56" s="10"/>
+      <c r="H56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10" t="s">
+      <c r="D57" s="9"/>
+      <c r="E57" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10" t="s">
+      <c r="F57" s="9"/>
+      <c r="G57" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="H57" s="10"/>
+      <c r="H57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10" t="s">
+      <c r="D58" s="9"/>
+      <c r="E58" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10" t="s">
+      <c r="F58" s="9"/>
+      <c r="G58" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="H58" s="10"/>
-    </row>
-    <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="H59" s="6"/>
-    </row>
+      <c r="H58" s="9"/>
+    </row>
+    <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11"/>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="10"/>
+      <c r="B60" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
     </row>
     <row r="61" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="11"/>
-      <c r="B61" s="8" t="s">
+      <c r="A61" s="10"/>
+      <c r="B61" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8" t="s">
+      <c r="D61" s="7"/>
+      <c r="E61" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8" t="s">
+      <c r="F61" s="7"/>
+      <c r="G61" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H61" s="8"/>
+      <c r="H61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11"/>
-      <c r="B62" s="9" t="s">
+      <c r="A62" s="10"/>
+      <c r="B62" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10" t="s">
+      <c r="D62" s="9"/>
+      <c r="E62" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10" t="s">
+      <c r="F62" s="9"/>
+      <c r="G62" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H62" s="10"/>
+      <c r="H62" s="9"/>
     </row>
     <row r="63" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="11"/>
-      <c r="B63" s="10" t="s">
+      <c r="A63" s="10"/>
+      <c r="B63" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10" t="s">
+      <c r="D63" s="9"/>
+      <c r="E63" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F63" s="10"/>
-      <c r="G63" s="10" t="s">
+      <c r="F63" s="9"/>
+      <c r="G63" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H63" s="10"/>
+      <c r="H63" s="9"/>
     </row>
     <row r="64" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="11"/>
-      <c r="B64" s="10" t="s">
+      <c r="A64" s="10"/>
+      <c r="B64" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10" t="s">
+      <c r="D64" s="9"/>
+      <c r="E64" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10" t="s">
+      <c r="F64" s="9"/>
+      <c r="G64" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="H64" s="10"/>
+      <c r="H64" s="9"/>
     </row>
     <row r="65" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="11"/>
-      <c r="B65" s="10" t="s">
+      <c r="A65" s="10"/>
+      <c r="B65" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10" t="s">
+      <c r="D65" s="9"/>
+      <c r="E65" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F65" s="10"/>
-      <c r="G65" s="10" t="s">
+      <c r="F65" s="9"/>
+      <c r="G65" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="H65" s="10"/>
+      <c r="H65" s="9"/>
     </row>
     <row r="66" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="11"/>
-      <c r="B66" s="10" t="s">
+      <c r="A66" s="10"/>
+      <c r="B66" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10" t="s">
+      <c r="D66" s="9"/>
+      <c r="E66" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F66" s="10"/>
-      <c r="G66" s="10" t="s">
+      <c r="F66" s="9"/>
+      <c r="G66" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H66" s="10"/>
+      <c r="H66" s="9"/>
     </row>
     <row r="67" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="11"/>
-      <c r="B67" s="10" t="s">
+      <c r="A67" s="10"/>
+      <c r="B67" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10" t="s">
+      <c r="D67" s="9"/>
+      <c r="E67" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10" t="s">
+      <c r="F67" s="9"/>
+      <c r="G67" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H67" s="10"/>
-    </row>
-    <row r="68" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="H68" s="6"/>
-    </row>
+      <c r="H67" s="9"/>
+    </row>
+    <row r="68" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0"/>
-      <c r="B69" s="8" t="s">
+      <c r="A69" s="11"/>
+      <c r="B69" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8" t="s">
+      <c r="C69" s="7"/>
+      <c r="D69" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8" t="s">
+      <c r="E69" s="7"/>
+      <c r="F69" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8" t="s">
+      <c r="G69" s="7"/>
+      <c r="H69" s="0"/>
+      <c r="I69" s="0"/>
+    </row>
+    <row r="70" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="11"/>
+      <c r="B70" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="I69" s="8"/>
-    </row>
-    <row r="70" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0"/>
-      <c r="B70" s="10" t="s">
+      <c r="C70" s="9"/>
+      <c r="D70" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10" t="s">
+      <c r="E70" s="9"/>
+      <c r="F70" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G70" s="9"/>
+      <c r="H70" s="0"/>
+      <c r="I70" s="0"/>
+    </row>
+    <row r="71" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="11"/>
+      <c r="B71" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10" t="s">
+      <c r="C71" s="9"/>
+      <c r="D71" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G71" s="9"/>
+      <c r="H71" s="0"/>
+      <c r="I71" s="0"/>
+    </row>
+    <row r="72" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="11"/>
+      <c r="B72" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I70" s="10"/>
-    </row>
-    <row r="71" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0"/>
-      <c r="B71" s="10" t="s">
+      <c r="C72" s="9"/>
+      <c r="D72" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G72" s="9"/>
+      <c r="H72" s="0"/>
+      <c r="I72" s="0"/>
+    </row>
+    <row r="73" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="11"/>
+      <c r="B73" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="I71" s="10"/>
-    </row>
-    <row r="72" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0"/>
-      <c r="B72" s="10" t="s">
+      <c r="C73" s="9"/>
+      <c r="D73" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G73" s="9"/>
+      <c r="H73" s="0"/>
+      <c r="I73" s="0"/>
+    </row>
+    <row r="74" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="11"/>
+      <c r="B74" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C72" s="10"/>
-      <c r="D72" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E72" s="10"/>
-      <c r="F72" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G72" s="10"/>
-      <c r="H72" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="I72" s="10"/>
-    </row>
-    <row r="73" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0"/>
-      <c r="B73" s="10" t="s">
+      <c r="C74" s="9"/>
+      <c r="D74" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G74" s="9"/>
+      <c r="H74" s="0"/>
+      <c r="I74" s="0"/>
+    </row>
+    <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="11"/>
+      <c r="B75" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="10"/>
-      <c r="D73" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G73" s="10"/>
-      <c r="H73" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I73" s="10"/>
-    </row>
-    <row r="74" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0"/>
-      <c r="B74" s="10" t="s">
+      <c r="C75" s="9"/>
+      <c r="D75" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G75" s="9"/>
+      <c r="H75" s="0"/>
+      <c r="I75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="11"/>
+      <c r="B76" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G74" s="10"/>
-      <c r="H74" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I74" s="10"/>
-    </row>
-    <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0"/>
-      <c r="B75" s="10" t="s">
+      <c r="C76" s="9"/>
+      <c r="D76" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G76" s="9"/>
+      <c r="H76" s="0"/>
+      <c r="I76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="11"/>
+      <c r="B77" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C75" s="10"/>
-      <c r="D75" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E75" s="10"/>
-      <c r="F75" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I75" s="10"/>
-    </row>
-    <row r="76" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0"/>
-      <c r="B76" s="10" t="s">
+      <c r="C77" s="9"/>
+      <c r="D77" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C76" s="10"/>
-      <c r="D76" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G76" s="10"/>
-      <c r="H76" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I76" s="10"/>
-    </row>
-    <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0"/>
-      <c r="B77" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10" t="s">
+      <c r="E77" s="9"/>
+      <c r="F77" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="I77" s="10"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="0"/>
+      <c r="I77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0"/>
+      <c r="A78" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="215">
+  <mergeCells count="206">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -7203,39 +7368,30 @@
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="D69:E69"/>
     <mergeCell ref="F69:G69"/>
-    <mergeCell ref="H69:I69"/>
     <mergeCell ref="B70:C70"/>
     <mergeCell ref="D70:E70"/>
     <mergeCell ref="F70:G70"/>
-    <mergeCell ref="H70:I70"/>
     <mergeCell ref="B71:C71"/>
     <mergeCell ref="D71:E71"/>
     <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="D72:E72"/>
     <mergeCell ref="F72:G72"/>
-    <mergeCell ref="H72:I72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:E73"/>
     <mergeCell ref="F73:G73"/>
-    <mergeCell ref="H73:I73"/>
     <mergeCell ref="B74:C74"/>
     <mergeCell ref="D74:E74"/>
     <mergeCell ref="F74:G74"/>
-    <mergeCell ref="H74:I74"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
     <mergeCell ref="B77:C77"/>
     <mergeCell ref="D77:E77"/>
     <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="1.025" header="0.511811023622047" footer="0.7875"/>
@@ -7245,4 +7401,336 @@
     <oddFooter>&amp;C&amp;K000000Page &amp;Kffffff&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="20.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="12" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new forms and controls, update project files
- Updated `BasicControls.csproj` to include `grpBox.cs` and `grpBox.Designer.cs`.
- Updated `MainForms.csproj` to include `frmAddFirm.cs`, `frmAddFirm.Designer.cs`, and `frmAddFirm.resx`.
- Updated `clInteractDb.cs` in `Models` to use `INSERT OR REPLACE` for `Users` and `INSERT OR IGNORE` for `States`.
- Added `grpBox.cs` and `grpBox.Designer.cs` for a custom `GroupBox` control in `BasicControls`.
- Added `frmAddFirm.cs` and `frmAddFirm.Designer.cs` for a new form in `MainForms`.
- Added `frmAddFirm.resx` for storing resources related to `frmAddFirm`.
</commit_message>
<xml_diff>
--- a/MediMax.xlsx
+++ b/MediMax.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="256">
   <si>
     <t xml:space="preserve">Sr.</t>
   </si>
@@ -365,9 +365,15 @@
     <t xml:space="preserve">Contact person's name.</t>
   </si>
   <si>
+    <t xml:space="preserve">AddA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Address line 1.</t>
   </si>
   <si>
+    <t xml:space="preserve">AddB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Address line 2.</t>
   </si>
   <si>
@@ -386,15 +392,27 @@
     <t xml:space="preserve">STD code (telephone).</t>
   </si>
   <si>
+    <t xml:space="preserve">LandLineA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Landline phone number 1.</t>
   </si>
   <si>
+    <t xml:space="preserve">LandLineB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Landline phone number 2.</t>
   </si>
   <si>
+    <t xml:space="preserve">MobNoA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mobile phone number 1.</t>
   </si>
   <si>
+    <t xml:space="preserve">MobNoB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mobile phone number 2.</t>
   </si>
   <si>
@@ -443,13 +461,25 @@
     <t xml:space="preserve">Expiry date for labour info.</t>
   </si>
   <si>
+    <t xml:space="preserve">DLNoA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drug License number 1.</t>
   </si>
   <si>
+    <t xml:space="preserve">DLExpA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expiry date for DL 1.</t>
   </si>
   <si>
+    <t xml:space="preserve">DLNoB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drug License number 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DLExpB</t>
   </si>
   <si>
     <t xml:space="preserve">Expiry date for DL 2.</t>
@@ -1070,7 +1100,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1119,11 +1149,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5966,10 +5992,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="25.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6248,6 +6274,10 @@
         <v>83</v>
       </c>
       <c r="H19" s="7"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="8" t="s">
@@ -6265,6 +6295,10 @@
         <v>86</v>
       </c>
       <c r="H20" s="9"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+      <c r="M20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
@@ -6282,6 +6316,10 @@
         <v>109</v>
       </c>
       <c r="H21" s="9"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="9" t="s">
@@ -6299,6 +6337,10 @@
         <v>110</v>
       </c>
       <c r="H22" s="9"/>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
+      <c r="M22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
@@ -6316,10 +6358,14 @@
         <v>112</v>
       </c>
       <c r="H23" s="9"/>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="9" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>87</v>
@@ -6330,13 +6376,17 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H24" s="9"/>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
+      <c r="M24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="9" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>87</v>
@@ -6347,9 +6397,13 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H25" s="9"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="9" t="s">
@@ -6364,9 +6418,13 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H26" s="9"/>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="9" t="s">
@@ -6381,9 +6439,13 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H27" s="9"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="9" t="s">
@@ -6394,13 +6456,17 @@
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H28" s="9"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="9" t="s">
@@ -6415,13 +6481,17 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H29" s="9"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="9" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>84</v>
@@ -6432,13 +6502,17 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H30" s="9"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="9" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>84</v>
@@ -6449,13 +6523,17 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="H31" s="9"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>45</v>
+        <v>126</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>84</v>
@@ -6466,13 +6544,17 @@
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="H32" s="9"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
+      <c r="M32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="9" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>84</v>
@@ -6483,9 +6565,13 @@
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H33" s="9"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
+      <c r="M33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="9" t="s">
@@ -6500,9 +6586,13 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H34" s="9"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="9" t="s">
@@ -6517,9 +6607,13 @@
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="H35" s="9"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
@@ -6534,9 +6628,13 @@
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H36" s="9"/>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
+      <c r="M36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="9" t="s">
@@ -6551,9 +6649,13 @@
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H37" s="9"/>
+      <c r="J37" s="0"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
+      <c r="M37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="9" t="s">
@@ -6568,9 +6670,13 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="H38" s="9"/>
+      <c r="J38" s="0"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
+      <c r="M38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="9" t="s">
@@ -6585,9 +6691,13 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H39" s="9"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="9" t="s">
@@ -6602,9 +6712,13 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H40" s="9"/>
+      <c r="J40" s="0"/>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="9" t="s">
@@ -6619,9 +6733,13 @@
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H41" s="9"/>
+      <c r="J41" s="0"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
+      <c r="M41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="9" t="s">
@@ -6636,9 +6754,13 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H42" s="9"/>
+      <c r="J42" s="0"/>
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
+      <c r="M42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="9" t="s">
@@ -6653,13 +6775,17 @@
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="H43" s="9"/>
+      <c r="J43" s="0"/>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="9" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>87</v>
@@ -6670,9 +6796,13 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H44" s="9"/>
+      <c r="J44" s="0"/>
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
+      <c r="M44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="9" t="s">
@@ -6687,9 +6817,13 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H45" s="9"/>
+      <c r="J45" s="0"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="9" t="s">
@@ -6704,9 +6838,13 @@
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="H46" s="9"/>
+      <c r="J46" s="0"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="9" t="s">
@@ -6721,13 +6859,17 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="H47" s="9"/>
+      <c r="J47" s="0"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="9" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>87</v>
@@ -6738,13 +6880,17 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="H48" s="9"/>
+      <c r="J48" s="0"/>
+      <c r="K48" s="0"/>
+      <c r="L48" s="0"/>
+      <c r="M48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="9" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>102</v>
@@ -6755,13 +6901,17 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H49" s="9"/>
+      <c r="J49" s="0"/>
+      <c r="K49" s="0"/>
+      <c r="L49" s="0"/>
+      <c r="M49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="9" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>87</v>
@@ -6772,13 +6922,17 @@
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="H50" s="9"/>
+      <c r="J50" s="0"/>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
+      <c r="M50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="9" t="s">
-        <v>65</v>
+        <v>151</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>102</v>
@@ -6789,9 +6943,13 @@
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="H51" s="9"/>
+      <c r="J51" s="0"/>
+      <c r="K51" s="0"/>
+      <c r="L51" s="0"/>
+      <c r="M51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="9" t="s">
@@ -6806,14 +6964,18 @@
       </c>
       <c r="F52" s="9"/>
       <c r="G52" s="9" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="H52" s="9"/>
+      <c r="J52" s="0"/>
+      <c r="K52" s="0"/>
+      <c r="L52" s="0"/>
+      <c r="M52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="6" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -6847,17 +7009,17 @@
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="9" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="H56" s="9"/>
     </row>
     <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="9" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>102</v>
@@ -6868,13 +7030,13 @@
       </c>
       <c r="F57" s="9"/>
       <c r="G57" s="9" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H57" s="9"/>
     </row>
     <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="9" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>102</v>
@@ -6885,7 +7047,7 @@
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="H58" s="9"/>
     </row>
@@ -6893,7 +7055,7 @@
     <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10"/>
       <c r="B60" s="6" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -6922,7 +7084,7 @@
     <row r="62" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="10"/>
       <c r="B62" s="8" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>84</v>
@@ -6947,11 +7109,11 @@
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="F63" s="9"/>
       <c r="G63" s="9" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="H63" s="9"/>
     </row>
@@ -6965,11 +7127,11 @@
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="9" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="F64" s="9"/>
       <c r="G64" s="9" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="H64" s="9"/>
     </row>
@@ -6983,11 +7145,11 @@
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="9" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="F65" s="9"/>
       <c r="G65" s="9" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="H65" s="9"/>
     </row>
@@ -7005,7 +7167,7 @@
       </c>
       <c r="F66" s="9"/>
       <c r="G66" s="9" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="H66" s="9"/>
     </row>
@@ -7023,7 +7185,7 @@
       </c>
       <c r="F67" s="9"/>
       <c r="G67" s="9" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="H67" s="9"/>
     </row>
@@ -7031,41 +7193,41 @@
     <row r="69" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="11"/>
       <c r="B69" s="7" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="G69" s="7"/>
-      <c r="H69" s="0"/>
-      <c r="I69" s="0"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
     </row>
     <row r="70" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="11"/>
       <c r="B70" s="9" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="9" t="s">
         <v>87</v>
       </c>
       <c r="G70" s="9"/>
-      <c r="H70" s="0"/>
-      <c r="I70" s="0"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="11"/>
       <c r="B71" s="9" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="C71" s="9"/>
       <c r="D71" s="9" t="s">
@@ -7076,13 +7238,13 @@
         <v>87</v>
       </c>
       <c r="G71" s="9"/>
-      <c r="H71" s="0"/>
-      <c r="I71" s="0"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
     </row>
     <row r="72" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="11"/>
       <c r="B72" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C72" s="9"/>
       <c r="D72" s="9" t="s">
@@ -7093,13 +7255,13 @@
         <v>102</v>
       </c>
       <c r="G72" s="9"/>
-      <c r="H72" s="0"/>
-      <c r="I72" s="0"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="11"/>
     </row>
     <row r="73" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="11"/>
       <c r="B73" s="9" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C73" s="9"/>
       <c r="D73" s="9" t="s">
@@ -7110,13 +7272,13 @@
         <v>104</v>
       </c>
       <c r="G73" s="9"/>
-      <c r="H73" s="0"/>
-      <c r="I73" s="0"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="11"/>
     </row>
     <row r="74" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="11"/>
       <c r="B74" s="9" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9" t="s">
@@ -7127,13 +7289,13 @@
         <v>91</v>
       </c>
       <c r="G74" s="9"/>
-      <c r="H74" s="0"/>
-      <c r="I74" s="0"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="11"/>
     </row>
     <row r="75" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="11"/>
       <c r="B75" s="9" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="9" t="s">
@@ -7144,42 +7306,42 @@
         <v>84</v>
       </c>
       <c r="G75" s="9"/>
-      <c r="H75" s="0"/>
-      <c r="I75" s="0"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="11"/>
     </row>
     <row r="76" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="11"/>
       <c r="B76" s="9" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="9" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="9" t="s">
         <v>84</v>
       </c>
       <c r="G76" s="9"/>
-      <c r="H76" s="0"/>
-      <c r="I76" s="0"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
     </row>
     <row r="77" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="11"/>
       <c r="B77" s="9" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="C77" s="9"/>
       <c r="D77" s="9" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="9" t="s">
         <v>95</v>
       </c>
       <c r="G77" s="9"/>
-      <c r="H77" s="0"/>
-      <c r="I77" s="0"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="11"/>
     </row>
     <row r="78" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="11"/>
@@ -7410,318 +7572,318 @@
   </sheetPr>
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="20.63"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="12" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="20.63"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="5" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>173</v>
+      <c r="A2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>175</v>
+      <c r="A3" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>177</v>
+      <c r="A4" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>179</v>
+      <c r="A5" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>181</v>
+      <c r="A6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>183</v>
+      <c r="A7" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>185</v>
+      <c r="A8" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>187</v>
+      <c r="A9" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>189</v>
+      <c r="A10" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>191</v>
+      <c r="A11" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>193</v>
+      <c r="A12" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>195</v>
+      <c r="A13" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>197</v>
+      <c r="A14" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>199</v>
+      <c r="A15" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>201</v>
+      <c r="A16" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>203</v>
+      <c r="A17" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>205</v>
+      <c r="A18" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>207</v>
+      <c r="A19" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>209</v>
+      <c r="A20" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>211</v>
+      <c r="A21" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>213</v>
+      <c r="A22" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>215</v>
+      <c r="A23" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>217</v>
+      <c r="A24" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>219</v>
+      <c r="A25" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>221</v>
+      <c r="A26" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>223</v>
+      <c r="A27" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>225</v>
+      <c r="A28" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>227</v>
+      <c r="A29" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>229</v>
+      <c r="A30" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>231</v>
+      <c r="A31" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>233</v>
+      <c r="A32" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>235</v>
+      <c r="A33" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>237</v>
+      <c r="A34" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>239</v>
+      <c r="A35" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>241</v>
+      <c r="A36" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>243</v>
+      <c r="A37" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>245</v>
+      <c r="A38" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>